<commit_message>
added code for experimentation
</commit_message>
<xml_diff>
--- a/cs534L-SAGmf.xlsx
+++ b/cs534L-SAGmf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Dataset</t>
   </si>
@@ -29,9 +29,6 @@
     <t>columns</t>
   </si>
   <si>
-    <t>epinions</t>
-  </si>
-  <si>
     <t>context</t>
   </si>
   <si>
@@ -44,18 +41,6 @@
     <t>SAG</t>
   </si>
   <si>
-    <t>99-percentile Best approximation</t>
-  </si>
-  <si>
-    <t>99-percentile running time (sec)</t>
-  </si>
-  <si>
-    <t>CLiMF</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>http://www.cise.ufl.edu/research/sparse/matrices/Gleich/wikipedia-20070206.html</t>
   </si>
   <si>
@@ -135,13 +120,49 @@
   </si>
   <si>
     <t>A(i,j)=1 if user i has tagged web page j as favorable, and a 0 represents no opinion.</t>
+  </si>
+  <si>
+    <t>epinions_train</t>
+  </si>
+  <si>
+    <t>epinions_test</t>
+  </si>
+  <si>
+    <t>https://github.com/gamboviol/climf</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>Best approximation</t>
+  </si>
+  <si>
+    <t>avg running time (sec) per iteration</t>
+  </si>
+  <si>
+    <t># of iterations</t>
+  </si>
+  <si>
+    <t>99.9-percentile (MB)</t>
+  </si>
+  <si>
+    <t>avg Memory (MB) per iteration</t>
+  </si>
+  <si>
+    <t>99.9-percentile (sec)</t>
+  </si>
+  <si>
+    <t>epinionsT</t>
+  </si>
+  <si>
+    <t>epinionsS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +181,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,7 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,14 +227,21 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -513,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,99 +579,96 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B2" s="6">
-        <v>3782463</v>
-      </c>
-      <c r="C2" s="6">
-        <v>428440</v>
-      </c>
-      <c r="D2" s="6">
-        <v>896308</v>
-      </c>
-      <c r="E2" s="6">
-        <v>21</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>32</v>
+        <v>23590</v>
+      </c>
+      <c r="C2" s="3">
+        <v>4718</v>
+      </c>
+      <c r="D2" s="3">
+        <v>49288</v>
+      </c>
+      <c r="E2" s="3">
+        <v>292</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B3" s="6">
-        <v>5021410</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2394385</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2394385</v>
-      </c>
-      <c r="E3" s="6">
-        <v>13</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>31</v>
+        <v>322445</v>
+      </c>
+      <c r="C3" s="3">
+        <v>4718</v>
+      </c>
+      <c r="D3" s="3">
+        <v>49288</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3935</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3782463</v>
+      </c>
+      <c r="C4" s="6">
+        <v>428440</v>
+      </c>
+      <c r="D4" s="6">
+        <v>896308</v>
+      </c>
+      <c r="E4" s="6">
+        <v>21</v>
+      </c>
+      <c r="F4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="6">
-        <v>5105039</v>
-      </c>
-      <c r="C4" s="6">
-        <v>916428</v>
-      </c>
-      <c r="D4" s="6">
-        <v>916428</v>
-      </c>
-      <c r="E4" s="6">
-        <v>16</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="6">
+        <v>5021410</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2394385</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2394385</v>
+      </c>
+      <c r="E5" s="6">
+        <v>13</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" s="6">
-        <v>5158388</v>
-      </c>
-      <c r="C5" s="6">
-        <v>735323</v>
-      </c>
-      <c r="D5" s="6">
-        <v>735323</v>
-      </c>
-      <c r="E5" s="6">
-        <v>9</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -644,16 +676,16 @@
         <v>24</v>
       </c>
       <c r="B6" s="6">
-        <v>9837214</v>
+        <v>5105039</v>
       </c>
       <c r="C6" s="6">
-        <v>820878</v>
+        <v>916428</v>
       </c>
       <c r="D6" s="6">
-        <v>820878</v>
+        <v>916428</v>
       </c>
       <c r="E6" s="6">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>23</v>
@@ -661,114 +693,152 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="6">
+        <v>5158388</v>
+      </c>
+      <c r="C7" s="6">
+        <v>735323</v>
+      </c>
+      <c r="D7" s="6">
+        <v>735323</v>
+      </c>
+      <c r="E7" s="6">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" s="6">
-        <v>16518948</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6">
+        <v>9837214</v>
+      </c>
+      <c r="C8" s="6">
+        <v>820878</v>
+      </c>
+      <c r="D8" s="6">
+        <v>820878</v>
+      </c>
+      <c r="E8" s="6">
+        <v>22</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="6">
+        <v>16518948</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="6">
+        <v>22624727</v>
+      </c>
+      <c r="C10" s="6">
+        <v>12471</v>
+      </c>
+      <c r="D10" s="6">
+        <v>872622</v>
+      </c>
+      <c r="E10" s="6">
         <v>36</v>
       </c>
-      <c r="B8" s="6">
-        <v>22624727</v>
-      </c>
-      <c r="C8" s="6">
-        <v>12471</v>
-      </c>
-      <c r="D8" s="6">
-        <v>872622</v>
-      </c>
-      <c r="E8" s="6">
-        <v>36</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="5">
+      <c r="F10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
         <v>45030389</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C11" s="6">
         <v>3566907</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D11" s="6">
         <v>3566907</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E11" s="6">
         <v>132</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="6">
+        <v>79023142</v>
+      </c>
+      <c r="C12" s="6">
+        <v>5363260</v>
+      </c>
+      <c r="D12" s="6">
+        <v>5363260</v>
+      </c>
+      <c r="E12" s="3">
+        <v>175</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="6">
-        <v>79023142</v>
-      </c>
-      <c r="C10" s="6">
-        <v>5363260</v>
-      </c>
-      <c r="D10" s="6">
-        <v>5363260</v>
-      </c>
-      <c r="E10" s="3">
-        <v>175</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="B13" s="6">
+        <v>1949412601</v>
+      </c>
+      <c r="C13" s="6">
+        <v>50636154</v>
+      </c>
+      <c r="D13" s="6">
+        <v>50636154</v>
+      </c>
+      <c r="E13" s="6">
+        <v>2483</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="6">
-        <v>1949412601</v>
-      </c>
-      <c r="C11" s="6">
-        <v>50636154</v>
-      </c>
-      <c r="D11" s="6">
-        <v>50636154</v>
-      </c>
-      <c r="E11" s="6">
-        <v>2483</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G13" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F14" s="10" t="s">
-        <v>38</v>
+      <c r="G14" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F15" s="9" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -776,7 +846,7 @@
     <sortCondition ref="B2:B14"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1" display="http://www.cise.ufl.edu/research/sparse/matrices/Gleich/wikipedia-20070206.html"/>
+    <hyperlink ref="A11" r:id="rId1" display="http://www.cise.ufl.edu/research/sparse/matrices/Gleich/wikipedia-20070206.html"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -784,67 +854,129 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="7" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" style="11" customWidth="1"/>
+    <col min="2" max="4" width="9.44140625" style="11" customWidth="1"/>
+    <col min="5" max="7" width="9" style="11" customWidth="1"/>
+    <col min="8" max="19" width="9.44140625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
+      <c r="H2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated path to data
</commit_message>
<xml_diff>
--- a/cs534L-SAGmf.xlsx
+++ b/cs534L-SAGmf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>http://www.cise.ufl.edu/research/sparse/matrices/Barabasi/NotreDame_actors.html</t>
   </si>
   <si>
-    <t>digg</t>
-  </si>
-  <si>
     <t>http://www.cise.ufl.edu/research/sparse/matrices/Buss/12month1.html</t>
   </si>
   <si>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>CLiMF/Win8.1</t>
+  </si>
+  <si>
+    <t>digg12month1</t>
   </si>
 </sst>
 </file>
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,12 +751,12 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="6">
         <v>23590</v>
@@ -771,12 +771,12 @@
         <v>292</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="6">
         <v>322445</v>
@@ -791,7 +791,7 @@
         <v>3935</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -913,7 +913,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
       <c r="B10" s="6">
         <v>22624727</v>
@@ -928,10 +928,10 @@
         <v>36</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1004,7 +1004,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F15" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1040,277 +1040,277 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
         <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
         <v>43</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
         <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
         <v>48</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>49</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>51</v>
-      </c>
-      <c r="B17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
         <v>67</v>
       </c>
-      <c r="B26" t="s">
-        <v>68</v>
-      </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" t="s">
         <v>70</v>
       </c>
-      <c r="B28" t="s">
-        <v>71</v>
-      </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
         <v>73</v>
       </c>
-      <c r="B31" t="s">
-        <v>74</v>
-      </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1334,32 +1334,32 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B1" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
       <c r="E1" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
       <c r="H1" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
       <c r="K1" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L1" s="17"/>
       <c r="M1" s="17"/>
       <c r="N1" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O1" s="17"/>
       <c r="P1" s="17"/>
       <c r="Q1" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R1" s="17"/>
       <c r="S1" s="17"/>
@@ -1372,65 +1372,65 @@
         <v>5</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -1440,12 +1440,12 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1465,7 +1465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1476,10 +1476,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
@@ -1493,23 +1493,23 @@
         <v>5</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1531,12 +1531,12 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated PPT and XLSX
</commit_message>
<xml_diff>
--- a/cs534L-SAGmf.xlsx
+++ b/cs534L-SAGmf.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="1" r:id="rId1"/>
-    <sheet name="parallel" sheetId="3" r:id="rId2"/>
-    <sheet name="CLiMF" sheetId="2" r:id="rId3"/>
-    <sheet name="memory" sheetId="4" r:id="rId4"/>
+    <sheet name="epinions" sheetId="5" r:id="rId2"/>
+    <sheet name="parallel" sheetId="3" r:id="rId3"/>
+    <sheet name="CLiMF" sheetId="2" r:id="rId4"/>
+    <sheet name="memory" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="106">
   <si>
     <t>Dataset</t>
   </si>
@@ -274,9 +275,6 @@
     <t>Wikipedia</t>
   </si>
   <si>
-    <t># of itrn @ convergence</t>
-  </si>
-  <si>
     <t>99%tile (sec) per itrn</t>
   </si>
   <si>
@@ -311,12 +309,44 @@
   </si>
   <si>
     <t>Memory (MB)</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>CLiMF</t>
+  </si>
+  <si>
+    <t>BPR</t>
+  </si>
+  <si>
+    <t>Stochastic</t>
+  </si>
+  <si>
+    <t>SAG lazy</t>
+  </si>
+  <si>
+    <t>Avg Time (sec) / itrn</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>99%tile Time (sec) / itrn</t>
+  </si>
+  <si>
+    <t># of itrns @ convergence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="3">
+    <numFmt numFmtId="169" formatCode="#,##0.0000000000000000"/>
+    <numFmt numFmtId="170" formatCode="0.0000000000000000E+00"/>
+    <numFmt numFmtId="171" formatCode="0.0000E+00"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -375,7 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -414,6 +444,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -723,7 +771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -920,7 +968,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="6">
         <v>22624727</v>
@@ -1032,6 +1080,135 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="20"/>
+    <col min="2" max="4" width="22.5546875" style="22" customWidth="1"/>
+    <col min="5" max="6" width="11.44140625" style="17" customWidth="1"/>
+    <col min="7" max="10" width="11.21875" style="24" customWidth="1"/>
+    <col min="11" max="16" width="8.88671875" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" s="26"/>
+      <c r="G1" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="J1" s="23"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="22">
+        <v>0.30537093783118802</v>
+      </c>
+      <c r="C3" s="22">
+        <v>0.30537059022623497</v>
+      </c>
+      <c r="D3" s="22">
+        <f>B3-C3</f>
+        <v>3.4760495304375638E-7</v>
+      </c>
+      <c r="E3" s="17">
+        <v>527</v>
+      </c>
+      <c r="F3" s="17">
+        <v>527</v>
+      </c>
+      <c r="G3" s="24">
+        <v>3.2486072899999899E-3</v>
+      </c>
+      <c r="H3" s="24">
+        <v>2.6417601933333302E-3</v>
+      </c>
+      <c r="I3" s="24">
+        <v>8.0864760000000004E-3</v>
+      </c>
+      <c r="J3" s="24">
+        <v>3.7554329999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="22">
+        <v>0.39336694517248899</v>
+      </c>
+      <c r="C4" s="22">
+        <v>0.39336456343380799</v>
+      </c>
+      <c r="D4" s="22">
+        <f t="shared" ref="D4:D7" si="0">B4-C4</f>
+        <v>2.3817386810009999E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D6" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="D7" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="E1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1325,12 +1502,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="E1" sqref="E1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1341,7 +1518,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="18" t="s">
         <v>36</v>
@@ -1349,27 +1526,27 @@
       <c r="C1" s="18"/>
       <c r="D1" s="18"/>
       <c r="E1" s="18" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="F1" s="18"/>
       <c r="G1" s="18"/>
       <c r="H1" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I1" s="18"/>
       <c r="J1" s="18"/>
       <c r="K1" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L1" s="18"/>
       <c r="M1" s="18"/>
       <c r="N1" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O1" s="18"/>
       <c r="P1" s="18"/>
       <c r="Q1" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R1" s="18"/>
       <c r="S1" s="18"/>
@@ -1385,7 +1562,7 @@
         <v>37</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>5</v>
@@ -1394,7 +1571,7 @@
         <v>37</v>
       </c>
       <c r="G2" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>5</v>
@@ -1403,7 +1580,7 @@
         <v>37</v>
       </c>
       <c r="J2" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>5</v>
@@ -1412,7 +1589,7 @@
         <v>37</v>
       </c>
       <c r="M2" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>5</v>
@@ -1421,7 +1598,7 @@
         <v>37</v>
       </c>
       <c r="P2" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -1430,7 +1607,7 @@
         <v>37</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -1471,7 +1648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -1486,10 +1663,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -1506,19 +1683,19 @@
         <v>37</v>
       </c>
       <c r="D2" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>95</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>96</v>
       </c>
       <c r="G2" t="s">
         <v>2</v>
       </c>
       <c r="H2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" t="s">
         <v>92</v>
-      </c>
-      <c r="I2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated PPTX and XLSX
</commit_message>
<xml_diff>
--- a/cs534L-SAGmf.xlsx
+++ b/cs534L-SAGmf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="12720" windowHeight="8016" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,15 @@
     <sheet name="parallel" sheetId="3" r:id="rId3"/>
     <sheet name="approx" sheetId="2" r:id="rId4"/>
     <sheet name="followUp" sheetId="6" r:id="rId5"/>
-    <sheet name="memory" sheetId="4" r:id="rId6"/>
+    <sheet name="full" sheetId="7" r:id="rId6"/>
+    <sheet name="memory" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="138">
   <si>
     <t>Dataset</t>
   </si>
@@ -321,9 +322,6 @@
     <t># of itrns @ convergence</t>
   </si>
   <si>
-    <t>SAG-A</t>
-  </si>
-  <si>
     <t>Sparse L2</t>
   </si>
   <si>
@@ -336,12 +334,6 @@
     <t>FG</t>
   </si>
   <si>
-    <t>SAG</t>
-  </si>
-  <si>
-    <t>SAG minus SG</t>
-  </si>
-  <si>
     <t>99.9%tile (sec) per itrn</t>
   </si>
   <si>
@@ -354,9 +346,6 @@
     <t>max itrns</t>
   </si>
   <si>
-    <t>DG</t>
-  </si>
-  <si>
     <t>non-zero's</t>
   </si>
   <si>
@@ -378,9 +367,6 @@
     <t>RAM (GB)</t>
   </si>
   <si>
-    <t>&gt; 5,000</t>
-  </si>
-  <si>
     <t>Digg*</t>
   </si>
   <si>
@@ -405,8 +391,11 @@
     <t>&gt; 36.00</t>
   </si>
   <si>
+    <t>SAG-MF</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">SAG time
+      <t xml:space="preserve">SAG-MF time
 </t>
     </r>
     <r>
@@ -419,6 +408,66 @@
       </rPr>
       <t>SG time</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SAG-MF time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+SG time</t>
+    </r>
+  </si>
+  <si>
+    <t>&gt; 58.00</t>
+  </si>
+  <si>
+    <t>&gt; 44.00</t>
+  </si>
+  <si>
+    <t>&gt; 46.00</t>
+  </si>
+  <si>
+    <t>&gt; 106.00</t>
+  </si>
+  <si>
+    <t>&gt; 118.00</t>
+  </si>
+  <si>
+    <t>&gt; 150.00</t>
+  </si>
+  <si>
+    <t>&gt; 48.00</t>
+  </si>
+  <si>
+    <t>&gt; 60.00</t>
+  </si>
+  <si>
+    <t>&gt; 70.00</t>
+  </si>
+  <si>
+    <t>re-com.</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t>SAG minus SG</t>
   </si>
 </sst>
 </file>
@@ -471,7 +520,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,6 +530,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,7 +553,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -569,6 +624,30 @@
     </xf>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -590,25 +669,10 @@
     <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -617,7 +681,9 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1228,7 +1294,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1241,23 +1307,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="38"/>
+      <c r="C1" s="50"/>
       <c r="D1" s="22"/>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="39" t="s">
+      <c r="F1" s="52"/>
+      <c r="G1" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39" t="s">
+      <c r="H1" s="51"/>
+      <c r="I1" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="39"/>
+      <c r="J1" s="51"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
@@ -1357,7 +1423,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1651,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1661,123 +1727,128 @@
     <col min="2" max="4" width="10.5546875" style="28" customWidth="1"/>
     <col min="5" max="5" width="12.44140625" style="28" customWidth="1"/>
     <col min="6" max="6" width="2.88671875" style="28" customWidth="1"/>
-    <col min="7" max="9" width="7.5546875" style="32" customWidth="1"/>
+    <col min="7" max="8" width="7.5546875" style="32" customWidth="1"/>
+    <col min="9" max="9" width="8.77734375" style="32" customWidth="1"/>
     <col min="10" max="10" width="2.21875" style="31" customWidth="1"/>
     <col min="11" max="11" width="7.6640625" style="24" customWidth="1"/>
     <col min="12" max="13" width="6.21875" style="24" customWidth="1"/>
     <col min="14" max="14" width="8.44140625" style="24" customWidth="1"/>
-    <col min="15" max="16" width="6.6640625" style="24" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" style="24" customWidth="1"/>
+    <col min="16" max="16" width="8.33203125" style="24" customWidth="1"/>
     <col min="17" max="17" width="2.109375" style="24" customWidth="1"/>
-    <col min="18" max="23" width="7" style="11" customWidth="1"/>
+    <col min="18" max="19" width="7" style="11" customWidth="1"/>
+    <col min="20" max="20" width="8" style="11" customWidth="1"/>
+    <col min="21" max="22" width="7" style="11" customWidth="1"/>
+    <col min="23" max="23" width="7.44140625" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="55" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
       <c r="J1" s="30"/>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44" t="s">
-        <v>107</v>
-      </c>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
       <c r="Q1" s="26"/>
-      <c r="R1" s="42" t="s">
+      <c r="R1" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="S1" s="42"/>
-      <c r="T1" s="42"/>
-      <c r="U1" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="V1" s="42"/>
-      <c r="W1" s="42"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" s="27" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="F2" s="27"/>
       <c r="G2" s="33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H2" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="33" t="s">
-        <v>100</v>
+      <c r="I2" s="44" t="s">
+        <v>123</v>
       </c>
       <c r="J2" s="30"/>
       <c r="K2" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L2" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="26" t="s">
-        <v>100</v>
+      <c r="M2" s="44" t="s">
+        <v>123</v>
       </c>
       <c r="N2" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O2" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="P2" s="26" t="s">
-        <v>100</v>
+      <c r="P2" s="44" t="s">
+        <v>123</v>
       </c>
       <c r="Q2" s="26"/>
       <c r="R2" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="S2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="T2" s="16" t="s">
-        <v>100</v>
+      <c r="T2" s="44" t="s">
+        <v>123</v>
       </c>
       <c r="U2" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="V2" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="W2" s="16" t="s">
-        <v>100</v>
+      <c r="W2" s="43" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B3" s="32"/>
       <c r="C3" s="32"/>
@@ -1810,13 +1881,13 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
     </row>
@@ -2094,11 +2165,11 @@
       <c r="A12" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
+      <c r="B12" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -2108,14 +2179,14 @@
         <v>-0.27529999999999999</v>
       </c>
       <c r="C13" s="28">
-        <v>-0.27350000000000002</v>
+        <v>-0.27353</v>
       </c>
       <c r="D13" s="28">
         <v>-0.2727</v>
       </c>
       <c r="E13" s="28">
         <f t="shared" si="0"/>
-        <v>8.0000000000002292E-4</v>
+        <v>8.2999999999999741E-4</v>
       </c>
       <c r="G13" s="32">
         <v>500</v>
@@ -2329,11 +2400,11 @@
       <c r="A19" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="41" t="s">
-        <v>102</v>
-      </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
+      <c r="B19" s="53" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="53"/>
+      <c r="D19" s="53"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
@@ -2580,82 +2651,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" style="25" customWidth="1"/>
-    <col min="3" max="4" width="11.109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="12" style="25" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="15" customWidth="1"/>
     <col min="5" max="6" width="14.21875" style="21" customWidth="1"/>
     <col min="7" max="8" width="14.6640625" style="15" customWidth="1"/>
-    <col min="9" max="10" width="14.6640625" style="25" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" style="54"/>
+    <col min="9" max="10" width="14.6640625" style="25" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="51" t="s">
-        <v>128</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="46" t="s">
-        <v>114</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="40" t="s">
+      <c r="B1" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="H1" s="40"/>
-      <c r="I1" s="48" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="52" t="s">
-        <v>128</v>
+      <c r="D1" s="58" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="51"/>
+      <c r="G1" s="52" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="52"/>
+      <c r="I1" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="61"/>
+      <c r="K1" s="59" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
       <c r="E2" s="20" t="s">
         <v>36</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="G2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="I2" s="49" t="s">
+      <c r="H2" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="K2" s="53"/>
+      <c r="J2" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="K2" s="60"/>
     </row>
     <row r="3" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="47" t="s">
-        <v>119</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="D3" s="38"/>
       <c r="G3" s="15">
         <v>20000</v>
       </c>
@@ -2668,16 +2738,16 @@
       <c r="J3" s="15">
         <v>5000</v>
       </c>
-      <c r="K3" s="54"/>
+      <c r="K3" s="41"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="F5" s="39"/>
+      <c r="F5" s="51"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
@@ -2688,12 +2758,12 @@
         <v>1.7586206896551726</v>
       </c>
       <c r="C6" s="15">
-        <f>MAX(0, approx!P6*approx!I6/approx!O6-approx!H6)</f>
-        <v>1877.8275862068976</v>
-      </c>
-      <c r="D6" s="15">
+        <f>MAX(0, (approx!P6*(approx!I6-1)+approx!N6)/approx!O6-approx!H6)</f>
+        <v>4597.0344827586214</v>
+      </c>
+      <c r="D6" s="45">
         <f>approx!H6+C6</f>
-        <v>4350.8275862068976</v>
+        <v>7070.0344827586214</v>
       </c>
       <c r="E6" s="21">
         <f>approx!C6</f>
@@ -2703,32 +2773,42 @@
         <f>approx!D6</f>
         <v>0.29260000000000003</v>
       </c>
+      <c r="G6" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H6" s="15">
         <f>approx!I6</f>
         <v>2474</v>
       </c>
+      <c r="I6" s="40" t="s">
+        <v>126</v>
+      </c>
       <c r="J6" s="25">
         <f>H6*approx!P6</f>
         <v>12.617400000000002</v>
       </c>
+      <c r="K6" s="41">
+        <f>J6/58</f>
+        <v>0.21754137931034487</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B7" s="25">
         <f>approx!M7/approx!L7</f>
         <v>1.3846153846153846</v>
       </c>
       <c r="C7" s="15">
-        <f>MAX(0, approx!M7*approx!I7/approx!L7-approx!H7)</f>
-        <v>5300.5384615384619</v>
-      </c>
-      <c r="D7" s="37">
+        <f>MAX(0, (approx!P7*(approx!I7-1)+approx!N7)/approx!O7-approx!H7)</f>
+        <v>4444.666666666667</v>
+      </c>
+      <c r="D7" s="45">
         <f>approx!H7+C7</f>
-        <v>6215.5384615384619</v>
-      </c>
-      <c r="E7" s="21">
+        <v>5359.666666666667</v>
+      </c>
+      <c r="E7" s="47">
         <f>approx!C7</f>
         <v>0.3125</v>
       </c>
@@ -2736,14 +2816,25 @@
         <f>approx!D7</f>
         <v>0.18809999999999999</v>
       </c>
+      <c r="G7" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H7" s="15">
         <f>approx!I7</f>
         <v>4489</v>
       </c>
+      <c r="I7" s="25">
+        <f>approx!O7*20000</f>
+        <v>47.999999999999993</v>
+      </c>
       <c r="J7" s="25">
         <f>H7*approx!P7</f>
         <v>10.773599999999998</v>
       </c>
+      <c r="K7" s="41">
+        <f>J7/48</f>
+        <v>0.22444999999999996</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="24" t="s">
@@ -2754,25 +2845,39 @@
         <v>1.5555555555555554</v>
       </c>
       <c r="C8" s="15">
-        <f>MAX(0, approx!P8*approx!I8/approx!O8-approx!H8)</f>
-        <v>2303.7777777777774</v>
-      </c>
-      <c r="D8" s="37">
+        <f>MAX(0, (approx!P8*(approx!I8-1)+approx!N8)/approx!O8-approx!H8)</f>
+        <v>3154.7777777777765</v>
+      </c>
+      <c r="D8" s="45">
         <f>approx!H8+C8</f>
-        <v>6447.7777777777774</v>
+        <v>7298.7777777777765</v>
+      </c>
+      <c r="E8" s="46">
+        <v>0.29777999999999999</v>
       </c>
       <c r="F8" s="21">
         <f>approx!D8</f>
         <v>0.29899999999999999</v>
       </c>
+      <c r="G8" s="37">
+        <v>5153</v>
+      </c>
       <c r="H8" s="15">
         <f>approx!I8</f>
         <v>4145</v>
       </c>
+      <c r="I8" s="25">
+        <f>approx!O8*G8</f>
+        <v>13.9131</v>
+      </c>
       <c r="J8" s="25">
         <f>H8*approx!P8</f>
         <v>17.408999999999999</v>
       </c>
+      <c r="K8" s="48">
+        <f>J8/I8</f>
+        <v>1.2512667917286586</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
@@ -2783,12 +2888,12 @@
         <v>1.4782608695652173</v>
       </c>
       <c r="C9" s="15">
-        <f>MAX(0, approx!P9*approx!I9/approx!O9-approx!H9)</f>
-        <v>143.99999999999977</v>
-      </c>
-      <c r="D9" s="15">
+        <f>MAX(0, (approx!P9*(approx!I9-1)+approx!N9)/approx!O9-approx!H9)</f>
+        <v>3196.478260869565</v>
+      </c>
+      <c r="D9" s="45">
         <f>approx!H9+C9</f>
-        <v>2005.9999999999998</v>
+        <v>5058.478260869565</v>
       </c>
       <c r="E9" s="21">
         <f>approx!C9</f>
@@ -2798,14 +2903,24 @@
         <f>approx!D9</f>
         <v>0.27789999999999998</v>
       </c>
+      <c r="G9" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H9" s="15">
         <f>approx!I9</f>
         <v>1357</v>
       </c>
+      <c r="I9" s="40" t="s">
+        <v>128</v>
+      </c>
       <c r="J9" s="25">
         <f>H9*approx!P9</f>
         <v>4.6137999999999995</v>
       </c>
+      <c r="K9" s="41">
+        <f>J9/46</f>
+        <v>0.10029999999999999</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
@@ -2816,14 +2931,14 @@
         <v>1.3636363636363635</v>
       </c>
       <c r="C10" s="15">
-        <f>MAX(0, approx!P10*approx!I10/approx!O10-approx!H10)</f>
-        <v>1403.545454545454</v>
-      </c>
-      <c r="D10" s="37">
+        <f>MAX(0, (approx!P10*(approx!I10-1)+approx!N10)/approx!O10-approx!H10)</f>
+        <v>3349.6818181818171</v>
+      </c>
+      <c r="D10" s="45">
         <f>approx!H10+C10</f>
-        <v>5259.545454545454</v>
-      </c>
-      <c r="E10" s="21">
+        <v>7205.6818181818171</v>
+      </c>
+      <c r="E10" s="47">
         <f>approx!C10</f>
         <v>0.30059999999999998</v>
       </c>
@@ -2831,26 +2946,37 @@
         <f>approx!D10</f>
         <v>0.26800000000000002</v>
       </c>
-      <c r="G10" s="47" t="s">
-        <v>124</v>
+      <c r="G10" s="38" t="s">
+        <v>119</v>
       </c>
       <c r="H10" s="15">
         <f>approx!I10</f>
         <v>3857</v>
       </c>
+      <c r="I10" s="40" t="s">
+        <v>127</v>
+      </c>
       <c r="J10" s="25">
         <f>H10*approx!P10</f>
         <v>11.571</v>
       </c>
+      <c r="K10" s="41">
+        <f>J10/44</f>
+        <v>0.26297727272727273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D11" s="45"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E12" s="39" t="s">
-        <v>103</v>
-      </c>
-      <c r="F12" s="39"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="51"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -2861,29 +2987,39 @@
         <v>2.358490566037736</v>
       </c>
       <c r="C13" s="15">
-        <f>MAX(0, approx!P13*approx!I13/approx!O13-approx!H13)</f>
-        <v>2538.6603773584911</v>
-      </c>
-      <c r="D13" s="15">
+        <f>MAX(0, (approx!P13*(approx!I13-1)+approx!N13)/approx!O13-approx!H13)</f>
+        <v>10270.396226415094</v>
+      </c>
+      <c r="D13" s="45">
         <f>approx!H13+C13</f>
-        <v>4405.6603773584911</v>
+        <v>12137.396226415094</v>
       </c>
       <c r="E13" s="21">
         <f>approx!C13</f>
-        <v>-0.27350000000000002</v>
+        <v>-0.27353</v>
       </c>
       <c r="F13" s="21">
         <f>approx!D13</f>
         <v>-0.2727</v>
       </c>
+      <c r="G13" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H13" s="15">
         <f>approx!I13</f>
         <v>1868</v>
       </c>
+      <c r="I13" s="40" t="s">
+        <v>129</v>
+      </c>
       <c r="J13" s="25">
         <f>H13*approx!P13</f>
         <v>23.35</v>
       </c>
+      <c r="K13" s="41">
+        <f>J13/106</f>
+        <v>0.22028301886792453</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
@@ -2894,12 +3030,12 @@
         <v>1.8135593220338984</v>
       </c>
       <c r="C14" s="15">
-        <f>MAX(0, approx!P14*approx!I14/approx!O14-approx!H14)</f>
-        <v>1209.9491525423728</v>
-      </c>
-      <c r="D14" s="15">
+        <f>MAX(0, (approx!P14*(approx!I14-1)+approx!N14)/approx!O14-approx!H14)</f>
+        <v>5221.0677966101703</v>
+      </c>
+      <c r="D14" s="45">
         <f>approx!H14+C14</f>
-        <v>2694.9491525423728</v>
+        <v>6706.0677966101703</v>
       </c>
       <c r="E14" s="21">
         <f>approx!C14</f>
@@ -2909,14 +3045,24 @@
         <f>approx!D14</f>
         <v>-1.0665</v>
       </c>
+      <c r="G14" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H14" s="15">
         <f>approx!I14</f>
         <v>1486</v>
       </c>
+      <c r="I14" s="40" t="s">
+        <v>130</v>
+      </c>
       <c r="J14" s="25">
         <f>H14*approx!P14</f>
         <v>15.9002</v>
       </c>
+      <c r="K14" s="41">
+        <f>J14/118</f>
+        <v>0.13474745762711865</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
@@ -2927,12 +3073,12 @@
         <v>1.4666666666666666</v>
       </c>
       <c r="C15" s="15">
-        <f>MAX(0, approx!P15*approx!I15/approx!O15-approx!H15)</f>
-        <v>117.19999999999999</v>
-      </c>
-      <c r="D15" s="15">
+        <f>MAX(0, (approx!P15*(approx!I15-1)+approx!N15)/approx!O15-approx!H15)</f>
+        <v>1255.4666666666667</v>
+      </c>
+      <c r="D15" s="49">
         <f>approx!H15+C15</f>
-        <v>365.2</v>
+        <v>1503.4666666666667</v>
       </c>
       <c r="E15" s="21">
         <f>approx!C15</f>
@@ -2942,14 +3088,24 @@
         <f>approx!D15</f>
         <v>-0.2712</v>
       </c>
+      <c r="G15" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H15" s="15">
         <f>approx!I15</f>
         <v>249</v>
       </c>
+      <c r="I15" s="40" t="s">
+        <v>131</v>
+      </c>
       <c r="J15" s="25">
         <f>H15*approx!P15</f>
         <v>2.7389999999999999</v>
       </c>
+      <c r="K15" s="41">
+        <f>J15/150</f>
+        <v>1.8259999999999998E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
@@ -2960,12 +3116,12 @@
         <v>1.9811320754716981</v>
       </c>
       <c r="C16" s="15">
-        <f>MAX(0, approx!P16*approx!I16/approx!O16-approx!H16)</f>
-        <v>900.69811320754729</v>
-      </c>
-      <c r="D16" s="15">
+        <f>MAX(0, (approx!P16*(approx!I16-1)+approx!N16)/approx!O16-approx!H16)</f>
+        <v>7890.4905660377353</v>
+      </c>
+      <c r="D16" s="45">
         <f>approx!H16+C16</f>
-        <v>1816.6981132075473</v>
+        <v>8806.4905660377353</v>
       </c>
       <c r="E16" s="21">
         <f>approx!C16</f>
@@ -2975,14 +3131,24 @@
         <f>approx!D16</f>
         <v>-0.27460000000000001</v>
       </c>
+      <c r="G16" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H16" s="15">
         <f>approx!I16</f>
         <v>917</v>
       </c>
+      <c r="I16" s="40" t="s">
+        <v>129</v>
+      </c>
       <c r="J16" s="25">
         <f>H16*approx!P16</f>
         <v>9.6285000000000007</v>
       </c>
+      <c r="K16" s="41">
+        <f>J16/106</f>
+        <v>9.0834905660377371E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
@@ -2993,48 +3159,52 @@
         <v>2.0526315789473681</v>
       </c>
       <c r="C17" s="15">
-        <f>MAX(0, approx!P17*approx!I17/approx!O17-approx!H17)</f>
-        <v>3643.105263157895</v>
-      </c>
-      <c r="D17" s="37">
+        <f>MAX(0, (approx!P17*(approx!I17-1)+approx!N17)/approx!O17-approx!H17)</f>
+        <v>9371.2368421052633</v>
+      </c>
+      <c r="D17" s="45">
         <f>approx!H17+C17</f>
-        <v>7102.105263157895</v>
+        <v>12830.236842105263</v>
       </c>
       <c r="E17" s="21">
-        <f>approx!C17</f>
-        <v>-0.2757</v>
+        <f>-0.275624157113277</f>
+        <v>-0.27562415711327698</v>
       </c>
       <c r="F17" s="21">
         <f>approx!D17</f>
         <v>-0.27379999999999999</v>
       </c>
-      <c r="G17" s="47" t="s">
-        <v>124</v>
+      <c r="G17" s="38" t="s">
+        <v>119</v>
       </c>
       <c r="H17" s="15">
         <f>approx!I17</f>
         <v>3460</v>
       </c>
-      <c r="I17" s="50" t="s">
-        <v>125</v>
+      <c r="I17" s="40" t="s">
+        <v>120</v>
       </c>
       <c r="J17" s="25">
         <f>H17*approx!P17</f>
         <v>26.988</v>
       </c>
-      <c r="K17" s="54">
+      <c r="K17" s="41">
         <f>J17/76</f>
         <v>0.35510526315789476</v>
       </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D18" s="45"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="39"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="51"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
@@ -3045,12 +3215,12 @@
         <v>2</v>
       </c>
       <c r="C20" s="15">
-        <f>MAX(0, approx!P20*approx!I20/approx!O20-approx!H20)</f>
-        <v>2489</v>
-      </c>
-      <c r="D20" s="15">
+        <f>MAX(0, (approx!P20*(approx!I20-1)+approx!N20)/approx!O20-approx!H20)</f>
+        <v>6172.3142857142866</v>
+      </c>
+      <c r="D20" s="45">
         <f>approx!H20+C20</f>
-        <v>4976</v>
+        <v>8659.3142857142866</v>
       </c>
       <c r="E20" s="21">
         <f>approx!C20</f>
@@ -3060,14 +3230,24 @@
         <f>approx!D20</f>
         <v>-7.0000000000000001E-3</v>
       </c>
+      <c r="G20" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H20" s="15">
         <f>approx!I20</f>
         <v>2488</v>
       </c>
+      <c r="I20" s="40" t="s">
+        <v>134</v>
+      </c>
       <c r="J20" s="25">
         <f>H20*approx!P20</f>
         <v>17.416</v>
       </c>
+      <c r="K20" s="41">
+        <f>J20/70</f>
+        <v>0.24879999999999999</v>
+      </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
@@ -3078,12 +3258,12 @@
         <v>1.1428571428571428</v>
       </c>
       <c r="C21" s="15">
-        <f>MAX(0, approx!P21*approx!I21/approx!O21-approx!H21)</f>
-        <v>687.57142857142844</v>
-      </c>
-      <c r="D21" s="37">
+        <f>MAX(0, (approx!P21*(approx!I21-1)+approx!N21)/approx!O21-approx!H21)</f>
+        <v>1943.1904761904761</v>
+      </c>
+      <c r="D21" s="45">
         <f>approx!H21+C21</f>
-        <v>5492.5714285714284</v>
+        <v>6748.1904761904761</v>
       </c>
       <c r="E21" s="21">
         <f>approx!C21</f>
@@ -3093,21 +3273,21 @@
         <f>approx!D21</f>
         <v>-1.41E-2</v>
       </c>
-      <c r="G21" s="47" t="s">
-        <v>124</v>
+      <c r="G21" s="38" t="s">
+        <v>119</v>
       </c>
       <c r="H21" s="15">
         <f>approx!I21</f>
         <v>4806</v>
       </c>
-      <c r="I21" s="50" t="s">
-        <v>126</v>
+      <c r="I21" s="40" t="s">
+        <v>121</v>
       </c>
       <c r="J21" s="25">
         <f>H21*approx!P21</f>
         <v>11.5344</v>
       </c>
-      <c r="K21" s="54">
+      <c r="K21" s="41">
         <f>J21/42</f>
         <v>0.27462857142857144</v>
       </c>
@@ -3121,12 +3301,12 @@
         <v>1.5666666666666667</v>
       </c>
       <c r="C22" s="15">
-        <f>MAX(0, approx!P22*approx!I22/approx!O22-approx!H22)</f>
-        <v>645.86666666666679</v>
-      </c>
-      <c r="D22" s="15">
+        <f>MAX(0, (approx!P22*(approx!I22-1)+approx!N22)/approx!O22-approx!H22)</f>
+        <v>1667.6</v>
+      </c>
+      <c r="D22" s="49">
         <f>approx!H22+C22</f>
-        <v>1782.8666666666668</v>
+        <v>2804.6</v>
       </c>
       <c r="E22" s="21">
         <f>approx!C22</f>
@@ -3136,14 +3316,24 @@
         <f>approx!D22</f>
         <v>-7.7000000000000002E-3</v>
       </c>
+      <c r="G22" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H22" s="15">
         <f>approx!I22</f>
         <v>1138</v>
       </c>
+      <c r="I22" s="40" t="s">
+        <v>133</v>
+      </c>
       <c r="J22" s="25">
         <f>H22*approx!P22</f>
         <v>5.3486000000000002</v>
       </c>
+      <c r="K22" s="41">
+        <f>J22/60</f>
+        <v>8.9143333333333338E-2</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
@@ -3154,10 +3344,10 @@
         <v>1.75</v>
       </c>
       <c r="C23" s="15">
-        <f>MAX(0, approx!P23*approx!I23/approx!O23-approx!H23)</f>
+        <f>MAX(0, (approx!P23*(approx!I23-1)+approx!N23)/approx!O23-approx!H23)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="15">
+      <c r="D23" s="49">
         <f>approx!H23+C23</f>
         <v>4838</v>
       </c>
@@ -3169,14 +3359,24 @@
         <f>approx!D23</f>
         <v>-6.4999999999999997E-3</v>
       </c>
+      <c r="G23" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="H23" s="15">
         <f>approx!I23</f>
         <v>470</v>
       </c>
+      <c r="I23" s="40" t="s">
+        <v>132</v>
+      </c>
       <c r="J23" s="25">
         <f>H23*approx!P23</f>
         <v>1.974</v>
       </c>
+      <c r="K23" s="41">
+        <f>J23/48</f>
+        <v>4.1125000000000002E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
@@ -3187,54 +3387,52 @@
         <v>1.8333333333333335</v>
       </c>
       <c r="C24" s="15">
-        <f>MAX(0, approx!P24*approx!I24/approx!O24-approx!H24)</f>
-        <v>3979.3333333333339</v>
-      </c>
-      <c r="D24" s="37">
+        <f>MAX(0, (approx!P24*(approx!I24-1)+approx!N24)/approx!O24-approx!H24)</f>
+        <v>6691.6111111111113</v>
+      </c>
+      <c r="D24" s="45">
         <f>approx!H24+C24</f>
-        <v>8752.3333333333339</v>
+        <v>11464.611111111111</v>
       </c>
       <c r="E24" s="21">
-        <f>approx!C24</f>
-        <v>-6.4000000000000003E-3</v>
+        <f>-0.007519276</f>
+        <v>-7.5192760000000001E-3</v>
       </c>
       <c r="F24" s="21">
         <f>approx!D24</f>
         <v>-0.03</v>
       </c>
-      <c r="G24" s="47" t="s">
-        <v>124</v>
+      <c r="G24" s="38" t="s">
+        <v>119</v>
       </c>
       <c r="H24" s="15">
         <f>approx!I24</f>
         <v>4774</v>
       </c>
-      <c r="I24" s="50" t="s">
-        <v>127</v>
+      <c r="I24" s="40" t="s">
+        <v>122</v>
       </c>
       <c r="J24" s="25">
         <f>H24*approx!P24</f>
         <v>15.754199999999999</v>
       </c>
-      <c r="K24" s="54">
+      <c r="K24" s="41">
         <f>J24/36</f>
         <v>0.43761666666666665</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="I1:J1"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E5:F5"/>
@@ -3243,6 +3441,8 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3251,16 +3451,29 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="5" width="6.21875" style="15" customWidth="1"/>
+    <col min="2" max="3" width="6.21875" style="15" customWidth="1"/>
+    <col min="4" max="5" width="7.44140625" style="15" customWidth="1"/>
     <col min="6" max="6" width="3.21875" customWidth="1"/>
     <col min="7" max="9" width="10.109375" style="15" customWidth="1"/>
   </cols>
@@ -3269,14 +3482,16 @@
       <c r="A1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="52"/>
       <c r="J1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -3284,16 +3499,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C2" s="35" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>2</v>
@@ -3302,7 +3517,7 @@
         <v>88</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -3483,8 +3698,8 @@
       <c r="C10" s="15">
         <v>1130</v>
       </c>
-      <c r="D10" s="47" t="s">
-        <v>116</v>
+      <c r="D10" s="38" t="s">
+        <v>112</v>
       </c>
       <c r="E10" s="15">
         <v>1141</v>
@@ -3509,8 +3724,8 @@
       <c r="C11" s="15">
         <v>865</v>
       </c>
-      <c r="D11" s="47" t="s">
-        <v>116</v>
+      <c r="D11" s="38" t="s">
+        <v>112</v>
       </c>
       <c r="E11" s="15">
         <v>880</v>
@@ -3535,8 +3750,8 @@
       <c r="C12" s="15">
         <v>2857</v>
       </c>
-      <c r="D12" s="47" t="s">
-        <v>116</v>
+      <c r="D12" s="38" t="s">
+        <v>112</v>
       </c>
       <c r="E12" s="15">
         <v>2944</v>
@@ -3561,8 +3776,8 @@
       <c r="C13" s="15">
         <v>2012</v>
       </c>
-      <c r="D13" s="47" t="s">
-        <v>116</v>
+      <c r="D13" s="38" t="s">
+        <v>112</v>
       </c>
       <c r="E13" s="15">
         <v>2069</v>
@@ -3582,15 +3797,16 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated intro and refs of paper
introduction.tex
refs.bib
</commit_message>
<xml_diff>
--- a/cs534L-SAGmf.xlsx
+++ b/cs534L-SAGmf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="12720" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="12720" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="1" r:id="rId1"/>
@@ -461,13 +461,13 @@
     <t>&gt; 70.00</t>
   </si>
   <si>
-    <t>re-com.</t>
-  </si>
-  <si>
     <t>generic</t>
   </si>
   <si>
     <t>SAG minus SG</t>
+  </si>
+  <si>
+    <t>ahead</t>
   </si>
 </sst>
 </file>
@@ -1717,21 +1717,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.77734375" style="11" customWidth="1"/>
     <col min="2" max="4" width="10.5546875" style="28" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="28" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="2.88671875" style="28" customWidth="1"/>
     <col min="7" max="8" width="7.5546875" style="32" customWidth="1"/>
     <col min="9" max="9" width="8.77734375" style="32" customWidth="1"/>
-    <col min="10" max="10" width="2.21875" style="31" customWidth="1"/>
-    <col min="11" max="11" width="7.6640625" style="24" customWidth="1"/>
-    <col min="12" max="13" width="6.21875" style="24" customWidth="1"/>
+    <col min="10" max="10" width="2.21875" style="31" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" style="24" hidden="1" customWidth="1"/>
+    <col min="12" max="13" width="6.21875" style="24" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="8.44140625" style="24" customWidth="1"/>
     <col min="15" max="15" width="6.6640625" style="24" customWidth="1"/>
     <col min="16" max="16" width="8.33203125" style="24" customWidth="1"/>
@@ -1795,7 +1795,7 @@
         <v>123</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F2" s="27"/>
       <c r="G2" s="33" t="s">
@@ -2651,7 +2651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -3433,16 +3433,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="K1:K2"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3466,7 +3466,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3505,10 +3505,10 @@
         <v>36</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
added tables to paper
</commit_message>
<xml_diff>
--- a/cs534L-SAGmf.xlsx
+++ b/cs534L-SAGmf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="12720" windowHeight="8016" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="12720" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="datasets" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="139">
   <si>
     <t>Dataset</t>
   </si>
@@ -373,9 +373,6 @@
     <t>*99%tile time are the same, so we used avg time to calculate multiplier</t>
   </si>
   <si>
-    <t>Given more time, i.e. an amount of time similar to SAG-A to account for re-computing, can SG yield an approximiation similar to or better than SAG?</t>
-  </si>
-  <si>
     <t>99%tile (sec) to reach better approx.</t>
   </si>
   <si>
@@ -394,8 +391,47 @@
     <t>SAG-MF</t>
   </si>
   <si>
+    <t>&gt; 58.00</t>
+  </si>
+  <si>
+    <t>&gt; 44.00</t>
+  </si>
+  <si>
+    <t>&gt; 46.00</t>
+  </si>
+  <si>
+    <t>&gt; 106.00</t>
+  </si>
+  <si>
+    <t>&gt; 118.00</t>
+  </si>
+  <si>
+    <t>&gt; 150.00</t>
+  </si>
+  <si>
+    <t>&gt; 48.00</t>
+  </si>
+  <si>
+    <t>&gt; 60.00</t>
+  </si>
+  <si>
+    <t>&gt; 70.00</t>
+  </si>
+  <si>
+    <t>generic</t>
+  </si>
+  <si>
+    <t>SAG minus SG</t>
+  </si>
+  <si>
+    <t>ahead</t>
+  </si>
+  <si>
+    <t>SAG-recomputed</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">SAG-MF time
+      <t xml:space="preserve">SAG-re. time
 </t>
     </r>
     <r>
@@ -419,7 +455,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>SAG-MF time</t>
+      <t>SAG-re. time</t>
     </r>
     <r>
       <rPr>
@@ -434,40 +470,7 @@
     </r>
   </si>
   <si>
-    <t>&gt; 58.00</t>
-  </si>
-  <si>
-    <t>&gt; 44.00</t>
-  </si>
-  <si>
-    <t>&gt; 46.00</t>
-  </si>
-  <si>
-    <t>&gt; 106.00</t>
-  </si>
-  <si>
-    <t>&gt; 118.00</t>
-  </si>
-  <si>
-    <t>&gt; 150.00</t>
-  </si>
-  <si>
-    <t>&gt; 48.00</t>
-  </si>
-  <si>
-    <t>&gt; 60.00</t>
-  </si>
-  <si>
-    <t>&gt; 70.00</t>
-  </si>
-  <si>
-    <t>generic</t>
-  </si>
-  <si>
-    <t>SAG minus SG</t>
-  </si>
-  <si>
-    <t>ahead</t>
+    <t>Given more time, i.e. an amount of time similar to SAG-re to account for re-computing, SG still could not yield an approximiation similar to or better than SAG in 14/15 cases.</t>
   </si>
 </sst>
 </file>
@@ -553,7 +556,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -648,6 +651,9 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1307,23 +1313,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="50"/>
+      <c r="C1" s="51"/>
       <c r="D1" s="22"/>
-      <c r="E1" s="52" t="s">
+      <c r="E1" s="53" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="51" t="s">
+      <c r="F1" s="53"/>
+      <c r="G1" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51" t="s">
+      <c r="H1" s="52"/>
+      <c r="I1" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="J1" s="51"/>
+      <c r="J1" s="52"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
@@ -1422,8 +1428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1718,7 +1724,7 @@
   <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1746,40 +1752,40 @@
       <c r="A1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
       <c r="E1" s="27"/>
       <c r="F1" s="27"/>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="56" t="s">
         <v>99</v>
       </c>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
       <c r="J1" s="30"/>
-      <c r="K1" s="56" t="s">
+      <c r="K1" s="57" t="s">
         <v>84</v>
       </c>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56" t="s">
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
+      <c r="N1" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="O1" s="56"/>
-      <c r="P1" s="56"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
       <c r="Q1" s="26"/>
-      <c r="R1" s="54" t="s">
+      <c r="R1" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54" t="s">
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55" t="s">
         <v>105</v>
       </c>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -1792,10 +1798,10 @@
         <v>36</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F2" s="27"/>
       <c r="G2" s="33" t="s">
@@ -1805,7 +1811,7 @@
         <v>36</v>
       </c>
       <c r="I2" s="44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J2" s="30"/>
       <c r="K2" s="27" t="s">
@@ -1815,7 +1821,7 @@
         <v>36</v>
       </c>
       <c r="M2" s="44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N2" s="27" t="s">
         <v>103</v>
@@ -1824,7 +1830,7 @@
         <v>36</v>
       </c>
       <c r="P2" s="44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q2" s="26"/>
       <c r="R2" s="27" t="s">
@@ -1834,7 +1840,7 @@
         <v>36</v>
       </c>
       <c r="T2" s="44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="U2" s="27" t="s">
         <v>103</v>
@@ -1843,7 +1849,7 @@
         <v>36</v>
       </c>
       <c r="W2" s="43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="15" customFormat="1" x14ac:dyDescent="0.3">
@@ -1883,11 +1889,11 @@
       <c r="A5" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="53" t="s">
+      <c r="B5" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
       <c r="E5" s="27"/>
       <c r="F5" s="27"/>
     </row>
@@ -2165,11 +2171,11 @@
       <c r="A12" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B12" s="53" t="s">
+      <c r="B12" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="53"/>
-      <c r="D12" s="53"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="54"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -2400,11 +2406,11 @@
       <c r="A19" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="53" t="s">
+      <c r="B19" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
@@ -2651,8 +2657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2671,55 +2677,55 @@
       <c r="A1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="57" t="s">
-        <v>125</v>
-      </c>
-      <c r="C1" s="58" t="s">
+      <c r="B1" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="52" t="s">
+      <c r="F1" s="52"/>
+      <c r="G1" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="52"/>
-      <c r="I1" s="61" t="s">
-        <v>118</v>
-      </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="59" t="s">
-        <v>124</v>
+      <c r="H1" s="53"/>
+      <c r="I1" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="J1" s="62"/>
+      <c r="K1" s="60" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
       <c r="E2" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="20" t="s">
-        <v>123</v>
+      <c r="F2" s="50" t="s">
+        <v>135</v>
       </c>
       <c r="G2" s="23" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I2" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="K2" s="60"/>
+      <c r="J2" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" s="61"/>
     </row>
     <row r="3" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
@@ -2744,10 +2750,10 @@
       <c r="A5" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="F5" s="51"/>
+      <c r="F5" s="52"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
@@ -2774,14 +2780,14 @@
         <v>0.29260000000000003</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H6" s="15">
         <f>approx!I6</f>
         <v>2474</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J6" s="25">
         <f>H6*approx!P6</f>
@@ -2817,15 +2823,14 @@
         <v>0.18809999999999999</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H7" s="15">
         <f>approx!I7</f>
         <v>4489</v>
       </c>
-      <c r="I7" s="25">
-        <f>approx!O7*20000</f>
-        <v>47.999999999999993</v>
+      <c r="I7" s="40" t="s">
+        <v>129</v>
       </c>
       <c r="J7" s="25">
         <f>H7*approx!P7</f>
@@ -2904,14 +2909,14 @@
         <v>0.27789999999999998</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H9" s="15">
         <f>approx!I9</f>
         <v>1357</v>
       </c>
       <c r="I9" s="40" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="J9" s="25">
         <f>H9*approx!P9</f>
@@ -2947,14 +2952,14 @@
         <v>0.26800000000000002</v>
       </c>
       <c r="G10" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H10" s="15">
         <f>approx!I10</f>
         <v>3857</v>
       </c>
       <c r="I10" s="40" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J10" s="25">
         <f>H10*approx!P10</f>
@@ -2973,10 +2978,10 @@
         <v>92</v>
       </c>
       <c r="D12" s="45"/>
-      <c r="E12" s="51" t="s">
+      <c r="E12" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="F12" s="51"/>
+      <c r="F12" s="52"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
@@ -3003,14 +3008,14 @@
         <v>-0.2727</v>
       </c>
       <c r="G13" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H13" s="15">
         <f>approx!I13</f>
         <v>1868</v>
       </c>
       <c r="I13" s="40" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J13" s="25">
         <f>H13*approx!P13</f>
@@ -3046,14 +3051,14 @@
         <v>-1.0665</v>
       </c>
       <c r="G14" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H14" s="15">
         <f>approx!I14</f>
         <v>1486</v>
       </c>
       <c r="I14" s="40" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="J14" s="25">
         <f>H14*approx!P14</f>
@@ -3089,14 +3094,14 @@
         <v>-0.2712</v>
       </c>
       <c r="G15" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H15" s="15">
         <f>approx!I15</f>
         <v>249</v>
       </c>
       <c r="I15" s="40" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J15" s="25">
         <f>H15*approx!P15</f>
@@ -3132,14 +3137,14 @@
         <v>-0.27460000000000001</v>
       </c>
       <c r="G16" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H16" s="15">
         <f>approx!I16</f>
         <v>917</v>
       </c>
       <c r="I16" s="40" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="J16" s="25">
         <f>H16*approx!P16</f>
@@ -3175,14 +3180,14 @@
         <v>-0.27379999999999999</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H17" s="15">
         <f>approx!I17</f>
         <v>3460</v>
       </c>
       <c r="I17" s="40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J17" s="25">
         <f>H17*approx!P17</f>
@@ -3201,10 +3206,10 @@
         <v>93</v>
       </c>
       <c r="D19" s="45"/>
-      <c r="E19" s="51" t="s">
+      <c r="E19" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="F19" s="51"/>
+      <c r="F19" s="52"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
@@ -3231,14 +3236,14 @@
         <v>-7.0000000000000001E-3</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H20" s="15">
         <f>approx!I20</f>
         <v>2488</v>
       </c>
       <c r="I20" s="40" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J20" s="25">
         <f>H20*approx!P20</f>
@@ -3274,14 +3279,14 @@
         <v>-1.41E-2</v>
       </c>
       <c r="G21" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H21" s="15">
         <f>approx!I21</f>
         <v>4806</v>
       </c>
       <c r="I21" s="40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J21" s="25">
         <f>H21*approx!P21</f>
@@ -3317,14 +3322,14 @@
         <v>-7.7000000000000002E-3</v>
       </c>
       <c r="G22" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H22" s="15">
         <f>approx!I22</f>
         <v>1138</v>
       </c>
       <c r="I22" s="40" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="J22" s="25">
         <f>H22*approx!P22</f>
@@ -3360,14 +3365,14 @@
         <v>-6.4999999999999997E-3</v>
       </c>
       <c r="G23" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H23" s="15">
         <f>approx!I23</f>
         <v>470</v>
       </c>
       <c r="I23" s="40" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J23" s="25">
         <f>H23*approx!P23</f>
@@ -3403,14 +3408,14 @@
         <v>-0.03</v>
       </c>
       <c r="G24" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H24" s="15">
         <f>approx!I24</f>
         <v>4774</v>
       </c>
       <c r="I24" s="40" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J24" s="25">
         <f>H24*approx!P24</f>
@@ -3423,7 +3428,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -3433,16 +3438,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="I1:J1"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3466,7 +3471,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3482,14 +3487,14 @@
       <c r="A1" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="52"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="53"/>
       <c r="J1" t="s">
         <v>114</v>
       </c>
@@ -3505,10 +3510,10 @@
         <v>36</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>2</v>

</xml_diff>